<commit_message>
<sc>commiting latest demo sheet
</commit_message>
<xml_diff>
--- a/CucumberFramework/src/test/resources/Data/DemoSprint.xlsx
+++ b/CucumberFramework/src/test/resources/Data/DemoSprint.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>RemoteAccess</t>
   </si>
@@ -41,37 +41,31 @@
     <t>OS</t>
   </si>
   <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>FreeDiskSpace</t>
-  </si>
-  <si>
     <t>NOCDefined</t>
   </si>
   <si>
-    <t>PartnerDefined</t>
-  </si>
-  <si>
-    <t>UserImpact</t>
-  </si>
-  <si>
-    <t>NonImpact</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>Alerts</t>
-  </si>
-  <si>
-    <t>Antivirus</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>wee</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>sxk</t>
+  </si>
+  <si>
+    <t>sdff</t>
+  </si>
+  <si>
+    <t>dfasdf</t>
   </si>
 </sst>
 </file>
@@ -389,106 +383,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>11</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-      <c r="N2">
-        <v>13</v>
-      </c>
-      <c r="O2">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>